<commit_message>
#282-Introduced Business Model 3
</commit_message>
<xml_diff>
--- a/Beelina.API/Templates/ReportTemplates/EndingInventoryPerProductReportAdmin_Template.xlsx
+++ b/Beelina.API/Templates/ReportTemplates/EndingInventoryPerProductReportAdmin_Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Beelina\Beelina.API\Templates\ReportTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A333DBF-7C4B-4B8D-A556-8EC00A6D83C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{459F3743-7688-4581-964A-315F2E3F55BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4BCE0149-8C23-4351-A0DE-0EABB1405EDD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Item Code</t>
   </si>
@@ -69,6 +69,12 @@
   </si>
   <si>
     <t>Warehouse Name:</t>
+  </si>
+  <si>
+    <t>Sold Stocks</t>
+  </si>
+  <si>
+    <t>Sold Stocks Value</t>
   </si>
 </sst>
 </file>
@@ -439,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FECBADA-66F2-4187-ACE2-9435ED0DBF8B}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,16 +460,18 @@
     <col min="6" max="6" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D1"/>
       <c r="F1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
@@ -471,7 +479,7 @@
       <c r="D2"/>
       <c r="F2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -479,7 +487,7 @@
       <c r="D3"/>
       <c r="F3"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -503,6 +511,12 @@
       </c>
       <c r="H5" s="7" t="s">
         <v>9</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>